<commit_message>
added miniscope triggering and improvements on plotting functions
</commit_message>
<xml_diff>
--- a/vr_tuning_params.xlsx
+++ b/vr_tuning_params.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,10 +448,10 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
4bit unity frame encoding
</commit_message>
<xml_diff>
--- a/vr_tuning_params.xlsx
+++ b/vr_tuning_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>notes</t>
   </si>
@@ -72,6 +72,24 @@
   </si>
   <si>
     <t>[180, 147.27, 114.54, 81.81, 49.09, 16.36, 0, -16.36, -49.09, -81.81, -114.54, -147.27]</t>
+  </si>
+  <si>
+    <t>[-90, 90]</t>
+  </si>
+  <si>
+    <t>[0.04444]</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>short2</t>
+  </si>
+  <si>
+    <t>head fixed</t>
+  </si>
+  <si>
+    <t>freely moving</t>
   </si>
 </sst>
 </file>
@@ -393,7 +411,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +423,7 @@
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -481,20 +499,96 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>

</xml_diff>

<commit_message>
more refinement on the vtuning and vwheel paradigms
</commit_message>
<xml_diff>
--- a/vr_tuning_params.xlsx
+++ b/vr_tuning_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>notes</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>freely moving</t>
+  </si>
+  <si>
+    <t>long free</t>
+  </si>
+  <si>
+    <t>shadow pause free</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,12 +597,50 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>

</xml_diff>

<commit_message>
added doric file conversion
</commit_message>
<xml_diff>
--- a/vr_tuning_params.xlsx
+++ b/vr_tuning_params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>notes</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>shadow pause free</t>
+  </si>
+  <si>
+    <t>anaesthetized</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,8 +646,27 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>

</xml_diff>